<commit_message>
Added four individual graphs need to fix
</commit_message>
<xml_diff>
--- a/OS Average Graph Calculation.xlsx
+++ b/OS Average Graph Calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryce\Desktop\OperatingSystemProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2397BB-3EE6-4892-A924-AA875ED054D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18E7A33-A079-4E0A-A2FF-D17A82D9C554}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18210" yWindow="0" windowWidth="20265" windowHeight="18960" xr2:uid="{121C1417-3774-44DC-AD81-C547B4B7BC59}"/>
+    <workbookView xWindow="18135" yWindow="0" windowWidth="20265" windowHeight="18960" xr2:uid="{121C1417-3774-44DC-AD81-C547B4B7BC59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>FCFS</t>
   </si>
@@ -840,7 +840,1239 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>35.133299999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>94.36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>178.578</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>291.214</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>430.71300000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>597.81299999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D67F-4049-B82D-E8B64DA48B91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="657524840"/>
+        <c:axId val="657525168"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="657524840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="657525168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="657525168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="657524840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>54.0533</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>155.62700000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>304.59100000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509.471</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>767.11599999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1078.1099999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7BA8-4D38-A278-71D94D356D61}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="611032000"/>
+        <c:axId val="611035608"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="611032000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="611035608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="611035608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="611032000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>54.3733</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>154.21299999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>302.80399999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>505.82799999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>764.06</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1073.54</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ECD7-438E-B7D4-82BEFD6CC5AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="615024424"/>
+        <c:axId val="615020160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="615024424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="615020160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="615020160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="615024424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>46.786700000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128.38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>247.87299999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>410.61</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>611.33799999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>848.298</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0B0B-441B-85DC-BDCEEE930185}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="615053456"/>
+        <c:axId val="616456584"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="615053456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="616456584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="616456584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="615053456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1383,6 +2615,2018 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1416,6 +4660,150 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>509587</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>204787</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B4305CF-B85D-45D1-A3B5-92510424C31F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>557212</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>252412</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B9C3D57-81F5-4D17-B091-6BA3358134B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>509587</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>204787</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E5593F1-84B3-4366-9CD7-EF9B40CA50A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A665D689-9127-4D5F-B733-AE72A6079117}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1723,8 +5111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAE96EA-8D4B-42FE-B6AB-DF15438614A6}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated the Graphs and added them to the document as well as the data
</commit_message>
<xml_diff>
--- a/OS Average Graph Calculation.xlsx
+++ b/OS Average Graph Calculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryce\Desktop\OperatingSystemProjects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brycecallender/Desktop/OperatingSystemProjects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18E7A33-A079-4E0A-A2FF-D17A82D9C554}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB342B4-0E41-084B-B48C-BF2D6657447D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18135" yWindow="0" windowWidth="20265" windowHeight="18960" xr2:uid="{121C1417-3774-44DC-AD81-C547B4B7BC59}"/>
+    <workbookView xWindow="13160" yWindow="460" windowWidth="12360" windowHeight="14460" xr2:uid="{121C1417-3774-44DC-AD81-C547B4B7BC59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>FCFS</t>
   </si>
@@ -855,6 +855,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SJF</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Scheduling Algorithm Turnaround Times</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -904,6 +934,33 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$3:$C$8</c:f>
@@ -957,6 +1014,67 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Jobs</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1021,6 +1139,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Turnaround</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1123,6 +1301,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>RR-2 Scheduling Algorithm Turnaround Times</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1172,6 +1380,33 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$3:$D$8</c:f>
@@ -1225,6 +1460,67 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Jobs</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1289,6 +1585,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Turnaround</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1391,6 +1747,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>RR-5 Scheduling Algorithm Turnaround Times</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1440,6 +1826,33 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$E$3:$E$8</c:f>
@@ -1493,6 +1906,67 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1050" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Number of Jobs</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1050">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1557,6 +2031,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Turnaround</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1659,6 +2193,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>FCFS</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Scheduling Algorithm Turnaround Times</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1708,6 +2271,33 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$3:$B$8</c:f>
@@ -1761,6 +2351,67 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Jobs</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1825,6 +2476,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Turnaround</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4632,15 +5343,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>395286</xdr:colOff>
+      <xdr:colOff>632353</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>185736</xdr:rowOff>
+      <xdr:rowOff>151870</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
+      <xdr:colOff>256116</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:rowOff>99483</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4669,14 +5380,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>509587</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>67203</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>204787</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:rowOff>139169</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4704,13 +5415,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>557212</xdr:colOff>
+      <xdr:colOff>574145</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>252412</xdr:colOff>
+      <xdr:colOff>269345</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
@@ -5111,13 +5822,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAE96EA-8D4B-42FE-B6AB-DF15438614A6}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5134,7 +5845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>5</v>
       </c>
@@ -5151,7 +5862,7 @@
         <v>54.3733</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>
@@ -5168,7 +5879,7 @@
         <v>154.21299999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>15</v>
       </c>
@@ -5185,7 +5896,7 @@
         <v>302.80399999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20</v>
       </c>
@@ -5202,7 +5913,7 @@
         <v>505.82799999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>25</v>
       </c>
@@ -5219,7 +5930,7 @@
         <v>764.06</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Talked about graphs and finished the word doc for now
</commit_message>
<xml_diff>
--- a/OS Average Graph Calculation.xlsx
+++ b/OS Average Graph Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brycecallender/Desktop/OperatingSystemProjects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB342B4-0E41-084B-B48C-BF2D6657447D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2025B4-9FBA-BC4A-B23F-F63A25B6807C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13160" yWindow="460" windowWidth="12360" windowHeight="14460" xr2:uid="{121C1417-3774-44DC-AD81-C547B4B7BC59}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5822,13 +5822,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CAE96EA-8D4B-42FE-B6AB-DF15438614A6}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="58" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5845,7 +5845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>5</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>54.3733</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>10</v>
       </c>
@@ -5879,7 +5879,7 @@
         <v>154.21299999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>15</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>302.80399999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>20</v>
       </c>
@@ -5913,7 +5913,7 @@
         <v>505.82799999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>25</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>764.06</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>30</v>
       </c>

</xml_diff>